<commit_message>
manipulating dataset and other fun stuff
</commit_message>
<xml_diff>
--- a/datasets/parks2.xlsx
+++ b/datasets/parks2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s2024589\Documents\course-repo\tutorial ideas\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s2024589\Documents\tutorial-kingakaszap\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -110,7 +110,7 @@
     <t>10 or more</t>
   </si>
   <si>
-    <t>5(could be morhen)</t>
+    <t>7(could be morhen)</t>
   </si>
 </sst>
 </file>
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -506,37 +506,55 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
       </c>
       <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="J2">
         <v>3</v>
       </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
+      <c r="K2">
+        <v>30</v>
       </c>
       <c r="L2">
         <v>4</v>
       </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
       <c r="O2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P2">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="Q2">
         <v>1</v>
       </c>
       <c r="R2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S2">
         <v>1</v>
@@ -582,19 +600,22 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="L4">
         <v>2</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
@@ -602,13 +623,13 @@
         <v>20</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -617,40 +638,49 @@
         <v>25</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
       </c>
       <c r="J5" t="s">
         <v>28</v>
       </c>
       <c r="K5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L5">
+        <v>7</v>
+      </c>
+      <c r="M5">
+        <v>7</v>
+      </c>
+      <c r="N5">
+        <v>8</v>
+      </c>
+      <c r="O5">
+        <v>8</v>
+      </c>
+      <c r="P5">
+        <v>8</v>
+      </c>
+      <c r="Q5">
+        <v>8</v>
+      </c>
+      <c r="R5">
+        <v>5</v>
+      </c>
+      <c r="S5">
         <v>6</v>
       </c>
-      <c r="M5">
-        <v>4</v>
-      </c>
-      <c r="N5">
-        <v>6</v>
-      </c>
-      <c r="O5">
-        <v>4</v>
-      </c>
-      <c r="P5">
-        <v>3</v>
-      </c>
-      <c r="Q5">
-        <v>5</v>
-      </c>
-      <c r="R5">
-        <v>4</v>
-      </c>
       <c r="T5">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="U5">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed initial dataset again
</commit_message>
<xml_diff>
--- a/datasets/parks2.xlsx
+++ b/datasets/parks2.xlsx
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>